<commit_message>
added code for arogya sanjeev  hospital cash  mediclassic outpatientcare starspecialcare youngstar
</commit_message>
<xml_diff>
--- a/src/test/java/Testdata/Testdata.xlsx
+++ b/src/test/java/Testdata/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="500" firstSheet="4" activeTab="9"/>
+    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="500" firstSheet="9" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="StarProduct" sheetId="2" r:id="rId1"/>
@@ -17,13 +17,19 @@
     <sheet name="cardiaccare" sheetId="10" r:id="rId8"/>
     <sheet name="cancergold" sheetId="11" r:id="rId9"/>
     <sheet name="fho" sheetId="12" r:id="rId10"/>
+    <sheet name="mediclassic" sheetId="13" r:id="rId11"/>
+    <sheet name="arogyasanjeev" sheetId="14" r:id="rId12"/>
+    <sheet name="specialcare" sheetId="15" r:id="rId13"/>
+    <sheet name="hospitalcash" sheetId="16" r:id="rId14"/>
+    <sheet name="outpatient" sheetId="17" r:id="rId15"/>
+    <sheet name="youngstar" sheetId="18" r:id="rId16"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="139">
   <si>
     <t>useremail</t>
   </si>
@@ -259,6 +265,9 @@
     <t>Outpatient Care</t>
   </si>
   <si>
+    <t>Myself and Others</t>
+  </si>
+  <si>
     <t>Young Star</t>
   </si>
   <si>
@@ -392,6 +401,51 @@
   </si>
   <si>
     <t>livein</t>
+  </si>
+  <si>
+    <t>productname</t>
+  </si>
+  <si>
+    <t>parentsyesorno</t>
+  </si>
+  <si>
+    <t>numofparents</t>
+  </si>
+  <si>
+    <t>parent1age</t>
+  </si>
+  <si>
+    <t>parent2age</t>
+  </si>
+  <si>
+    <t>parent3age</t>
+  </si>
+  <si>
+    <t>parent4age</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>4,00,000</t>
+  </si>
+  <si>
+    <t>plantype</t>
+  </si>
+  <si>
+    <t>coveragedays</t>
+  </si>
+  <si>
+    <t>Enhanced</t>
+  </si>
+  <si>
+    <t>numofmembers</t>
+  </si>
+  <si>
+    <t>GOLD</t>
+  </si>
+  <si>
+    <t>5,00,000</t>
   </si>
 </sst>
 </file>
@@ -1139,13 +1193,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1156,6 +1210,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
@@ -1489,8 +1544,8 @@
   <sheetPr/>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -1576,21 +1631,21 @@
       <c r="Q1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="R1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="S1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="T1" s="26" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -1602,7 +1657,7 @@
       <c r="E2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="24">
         <v>30</v>
       </c>
       <c r="G2" s="11" t="s">
@@ -1623,13 +1678,13 @@
       <c r="L2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="25" t="s">
         <v>29</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="24" t="s">
+      <c r="O2" s="25" t="s">
         <v>31</v>
       </c>
       <c r="P2" s="11">
@@ -1664,8 +1719,8 @@
   <sheetPr/>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -1700,7 +1755,7 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>8</v>
@@ -1732,10 +1787,10 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>55</v>
@@ -1753,10 +1808,10 @@
         <v>500072</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J2" s="1">
         <v>500072</v>
@@ -1765,13 +1820,13 @@
         <v>53</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="O2" s="1">
         <v>2021</v>
@@ -1780,6 +1835,994 @@
         <v>123</v>
       </c>
     </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="sangeethanulu@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:S9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="22.6" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="4" width="26.3" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="7" max="8" width="14.6" customWidth="1"/>
+    <col min="9" max="9" width="16.7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1">
+        <v>56</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="1">
+        <v>500072</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M2" s="1">
+        <v>500072</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R2" s="1">
+        <v>2021</v>
+      </c>
+      <c r="S2" s="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="sangeethanulu@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:X9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="22.6" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="5" width="26.3" customWidth="1"/>
+    <col min="7" max="12" width="15.2" customWidth="1"/>
+    <col min="13" max="13" width="16.7" customWidth="1"/>
+    <col min="14" max="14" width="7.6" customWidth="1"/>
+    <col min="15" max="15" width="18.5" customWidth="1"/>
+    <col min="17" max="18" width="11.4" customWidth="1"/>
+    <col min="20" max="20" width="14" customWidth="1"/>
+    <col min="22" max="22" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="1">
+        <v>56</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1">
+        <v>65</v>
+      </c>
+      <c r="J2" s="1">
+        <v>65</v>
+      </c>
+      <c r="K2" s="1">
+        <v>65</v>
+      </c>
+      <c r="L2" s="1">
+        <v>65</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="N2" s="1">
+        <v>600000</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1254</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="S2" s="1">
+        <v>500072</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="U2" s="1">
+        <v>38</v>
+      </c>
+      <c r="V2" s="1">
+        <v>100</v>
+      </c>
+      <c r="W2" s="1">
+        <v>169</v>
+      </c>
+      <c r="X2" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1"/>
+    <row r="4" customFormat="1"/>
+    <row r="5" customFormat="1"/>
+    <row r="6" customFormat="1"/>
+    <row r="7" customFormat="1"/>
+    <row r="8" customFormat="1"/>
+    <row r="9" customFormat="1" ht="15" customHeight="1"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="sangeethanulu@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="22.6" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="4" width="26.3" customWidth="1"/>
+    <col min="6" max="6" width="13.9" customWidth="1"/>
+    <col min="7" max="7" width="16.7" customWidth="1"/>
+    <col min="8" max="8" width="7.6" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="11" max="12" width="11.4" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="16" max="16" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1">
+        <v>600000</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1254</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M2" s="1">
+        <v>500072</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O2" s="1">
+        <v>38</v>
+      </c>
+      <c r="P2" s="1">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>169</v>
+      </c>
+      <c r="R2" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1"/>
+    <row r="4" customFormat="1"/>
+    <row r="5" customFormat="1"/>
+    <row r="6" customFormat="1"/>
+    <row r="7" customFormat="1"/>
+    <row r="8" customFormat="1"/>
+    <row r="9" customFormat="1" ht="15" customHeight="1"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="sangeethanulu@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:U9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="22.6" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="5" width="26.3" customWidth="1"/>
+    <col min="7" max="7" width="10.1" customWidth="1"/>
+    <col min="8" max="8" width="13.9" customWidth="1"/>
+    <col min="9" max="10" width="16.7" customWidth="1"/>
+    <col min="11" max="11" width="7.6" customWidth="1"/>
+    <col min="12" max="12" width="18.5" customWidth="1"/>
+    <col min="14" max="15" width="11.4" customWidth="1"/>
+    <col min="17" max="17" width="14" customWidth="1"/>
+    <col min="19" max="19" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="3">
+        <v>3000</v>
+      </c>
+      <c r="J2" s="3">
+        <v>90</v>
+      </c>
+      <c r="K2" s="1">
+        <v>600000</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1254</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="P2" s="1">
+        <v>500072</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="R2" s="1">
+        <v>38</v>
+      </c>
+      <c r="S2" s="1">
+        <v>100</v>
+      </c>
+      <c r="T2" s="1">
+        <v>169</v>
+      </c>
+      <c r="U2" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1"/>
+    <row r="4" customFormat="1"/>
+    <row r="5" customFormat="1"/>
+    <row r="6" customFormat="1"/>
+    <row r="7" customFormat="1"/>
+    <row r="8" customFormat="1"/>
+    <row r="9" customFormat="1" ht="15" customHeight="1"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="sangeethanulu@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:U9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="22.6" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="5" width="26.3" customWidth="1"/>
+    <col min="7" max="8" width="14.6" customWidth="1"/>
+    <col min="9" max="9" width="13.3" customWidth="1"/>
+    <col min="10" max="10" width="16.7" customWidth="1"/>
+    <col min="11" max="11" width="7.6" customWidth="1"/>
+    <col min="12" max="12" width="18.5" customWidth="1"/>
+    <col min="14" max="15" width="11.4" customWidth="1"/>
+    <col min="17" max="17" width="14" customWidth="1"/>
+    <col min="19" max="19" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="3">
+        <v>50000</v>
+      </c>
+      <c r="K2" s="1">
+        <v>600000</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1254</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="P2" s="1">
+        <v>500072</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="R2" s="1">
+        <v>38</v>
+      </c>
+      <c r="S2" s="1">
+        <v>100</v>
+      </c>
+      <c r="T2" s="1">
+        <v>169</v>
+      </c>
+      <c r="U2" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1"/>
+    <row r="4" customFormat="1"/>
+    <row r="5" customFormat="1"/>
+    <row r="6" customFormat="1"/>
+    <row r="7" customFormat="1"/>
+    <row r="8" customFormat="1"/>
+    <row r="9" customFormat="1" ht="15" customHeight="1"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="sangeethanulu@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="22.6" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="5" width="26.3" customWidth="1"/>
+    <col min="7" max="8" width="13.3" customWidth="1"/>
+    <col min="9" max="9" width="16.7" customWidth="1"/>
+    <col min="10" max="10" width="7.6" customWidth="1"/>
+    <col min="11" max="11" width="18.5" customWidth="1"/>
+    <col min="13" max="14" width="11.4" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
+    <col min="18" max="18" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="1">
+        <v>40</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J2" s="1">
+        <v>600000</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1254</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="O2" s="1">
+        <v>500072</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>38</v>
+      </c>
+      <c r="R2" s="1">
+        <v>100</v>
+      </c>
+      <c r="S2" s="1">
+        <v>169</v>
+      </c>
+      <c r="T2" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1"/>
+    <row r="4" customFormat="1"/>
+    <row r="5" customFormat="1"/>
+    <row r="6" customFormat="1"/>
+    <row r="7" customFormat="1"/>
+    <row r="8" customFormat="1"/>
+    <row r="9" customFormat="1" ht="15" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="sangeethanulu@gmail.com"/>
@@ -1814,75 +2857,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:73">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="BH1" s="20"/>
-      <c r="BI1" s="20"/>
-      <c r="BJ1" s="20"/>
-      <c r="BK1" s="20"/>
-      <c r="BL1" s="20"/>
-      <c r="BM1" s="20"/>
-      <c r="BN1" s="20"/>
-      <c r="BO1" s="20"/>
-      <c r="BP1" s="20"/>
-      <c r="BQ1" s="20"/>
-      <c r="BR1" s="20"/>
-      <c r="BS1" s="20"/>
-      <c r="BT1" s="20"/>
-      <c r="BU1" s="20"/>
+      <c r="BH1" s="21"/>
+      <c r="BI1" s="21"/>
+      <c r="BJ1" s="21"/>
+      <c r="BK1" s="21"/>
+      <c r="BL1" s="21"/>
+      <c r="BM1" s="21"/>
+      <c r="BN1" s="21"/>
+      <c r="BO1" s="21"/>
+      <c r="BP1" s="21"/>
+      <c r="BQ1" s="21"/>
+      <c r="BR1" s="21"/>
+      <c r="BS1" s="21"/>
+      <c r="BT1" s="21"/>
+      <c r="BU1" s="21"/>
     </row>
     <row r="2" ht="16.35" spans="1:73">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="16">
         <v>9533679769</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="AA2" s="18"/>
-      <c r="AL2" s="19"/>
-      <c r="AP2" s="18"/>
-      <c r="BH2" s="21"/>
-      <c r="BI2" s="21"/>
-      <c r="BJ2" s="21"/>
-      <c r="BK2" s="21"/>
-      <c r="BL2" s="21"/>
-      <c r="BM2" s="21"/>
-      <c r="BN2" s="21"/>
-      <c r="BO2" s="21"/>
-      <c r="BP2" s="21"/>
-      <c r="BQ2" s="21"/>
-      <c r="BR2" s="21"/>
-      <c r="BS2" s="21"/>
-      <c r="BT2" s="21"/>
-      <c r="BU2" s="21"/>
+      <c r="AA2" s="19"/>
+      <c r="AL2" s="20"/>
+      <c r="AP2" s="19"/>
+      <c r="BH2" s="22"/>
+      <c r="BI2" s="22"/>
+      <c r="BJ2" s="22"/>
+      <c r="BK2" s="22"/>
+      <c r="BL2" s="22"/>
+      <c r="BM2" s="22"/>
+      <c r="BN2" s="22"/>
+      <c r="BO2" s="22"/>
+      <c r="BP2" s="22"/>
+      <c r="BQ2" s="22"/>
+      <c r="BR2" s="22"/>
+      <c r="BS2" s="22"/>
+      <c r="BT2" s="22"/>
+      <c r="BU2" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1902,7 +2945,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelCol="6"/>
@@ -2163,7 +3206,9 @@
       <c r="A18" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -2171,10 +3216,10 @@
       <c r="G18" s="11"/>
     </row>
     <row r="19" ht="16.35" spans="1:7">
-      <c r="A19" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="14"/>
+      <c r="A19" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="15"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -2194,10 +3239,18 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:P2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="22.6" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="16.7" customWidth="1"/>
+    <col min="7" max="7" width="13.9" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
@@ -2251,10 +3304,10 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>48</v>
@@ -2272,10 +3325,10 @@
         <v>50</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J2" s="1">
         <v>500072</v>
@@ -2284,13 +3337,13 @@
         <v>53</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="O2" s="1">
         <v>2021</v>
@@ -2314,7 +3367,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:Q2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2336,10 +3389,10 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -2374,10 +3427,10 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>62</v>
@@ -2389,19 +3442,19 @@
         <v>25</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K2" s="1">
         <v>500072</v>
@@ -2410,13 +3463,13 @@
         <v>53</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="P2" s="1">
         <v>2021</v>
@@ -2440,7 +3493,7 @@
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:V2"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2456,81 +3509,81 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="3" t="s">
-        <v>79</v>
+      <c r="A2" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E2" s="1">
         <v>65</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>24</v>
@@ -2539,23 +3592,23 @@
         <v>600000</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J2" s="1">
         <v>1658</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N2" s="1">
         <v>500072</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="P2" s="1">
         <v>43</v>
@@ -2613,54 +3666,54 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="3" t="s">
-        <v>79</v>
+      <c r="A2" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>60</v>
@@ -2669,34 +3722,34 @@
         <v>56</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="3">
         <v>42000</v>
       </c>
       <c r="H2" s="1">
         <v>600000</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J2" s="1">
         <v>1254</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M2" s="1">
         <v>500072</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="O2" s="1">
         <v>38</v>
@@ -2726,7 +3779,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:Q2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2745,51 +3798,51 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="3" t="s">
-        <v>79</v>
+      <c r="A2" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -2807,22 +3860,22 @@
         <v>600000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I2" s="1">
         <v>1254</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L2" s="1">
         <v>500072</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N2" s="1">
         <v>38</v>
@@ -2871,60 +3924,60 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="3" t="s">
-        <v>79</v>
+      <c r="A2" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>68</v>
@@ -2933,7 +3986,7 @@
         <v>59</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>33</v>
@@ -2942,22 +3995,22 @@
         <v>600000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I2" s="1">
         <v>1254</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L2" s="1">
         <v>500072</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N2" s="1">
         <v>38</v>
@@ -2972,13 +4025,13 @@
         <v>62</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="S2" s="4">
+        <v>121</v>
+      </c>
+      <c r="S2" s="5">
         <v>44102</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added code for star care micro insurance policy, star criticare plus insurance policy,star family delite,star micro rural products
</commit_message>
<xml_diff>
--- a/src/test/java/Testdata/Testdata.xlsx
+++ b/src/test/java/Testdata/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="500" firstSheet="9" activeTab="15"/>
+    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="500" firstSheet="13" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="StarProduct" sheetId="2" r:id="rId1"/>
@@ -23,13 +23,17 @@
     <sheet name="hospitalcash" sheetId="16" r:id="rId14"/>
     <sheet name="outpatient" sheetId="17" r:id="rId15"/>
     <sheet name="youngstar" sheetId="18" r:id="rId16"/>
+    <sheet name="SCMIP" sheetId="19" r:id="rId17"/>
+    <sheet name="SCCPP" sheetId="20" r:id="rId18"/>
+    <sheet name="SFDIP" sheetId="21" r:id="rId19"/>
+    <sheet name="microrural" sheetId="22" r:id="rId20"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="141">
   <si>
     <t>useremail</t>
   </si>
@@ -406,6 +410,9 @@
     <t>productname</t>
   </si>
   <si>
+    <t>numofkids</t>
+  </si>
+  <si>
     <t>parentsyesorno</t>
   </si>
   <si>
@@ -446,6 +453,9 @@
   </si>
   <si>
     <t>5,00,000</t>
+  </si>
+  <si>
+    <t>2 Lakhs</t>
   </si>
 </sst>
 </file>
@@ -1544,7 +1554,7 @@
   <sheetPr/>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -1720,7 +1730,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -1796,7 +1806,7 @@
         <v>55</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1">
         <v>25</v>
@@ -1994,10 +2004,10 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>
@@ -2005,16 +2015,16 @@
     <col min="1" max="1" width="22.6" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="5" width="26.3" customWidth="1"/>
-    <col min="7" max="12" width="15.2" customWidth="1"/>
-    <col min="13" max="13" width="16.7" customWidth="1"/>
-    <col min="14" max="14" width="7.6" customWidth="1"/>
-    <col min="15" max="15" width="18.5" customWidth="1"/>
-    <col min="17" max="18" width="11.4" customWidth="1"/>
-    <col min="20" max="20" width="14" customWidth="1"/>
-    <col min="22" max="22" width="10.5" customWidth="1"/>
+    <col min="8" max="13" width="15.2" customWidth="1"/>
+    <col min="14" max="14" width="16.7" customWidth="1"/>
+    <col min="15" max="15" width="7.6" customWidth="1"/>
+    <col min="16" max="16" width="18.5" customWidth="1"/>
+    <col min="18" max="19" width="11.4" customWidth="1"/>
+    <col min="21" max="21" width="14" customWidth="1"/>
+    <col min="23" max="23" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2052,43 +2062,46 @@
         <v>130</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:25">
       <c r="A2" s="2" t="s">
         <v>80</v>
       </c>
@@ -2102,19 +2115,19 @@
         <v>70</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F2" s="1">
         <v>56</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H2" s="1">
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="1">
         <v>2</v>
-      </c>
-      <c r="I2" s="1">
-        <v>65</v>
       </c>
       <c r="J2" s="1">
         <v>65</v>
@@ -2125,40 +2138,43 @@
       <c r="L2" s="1">
         <v>65</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="N2" s="1">
+      <c r="M2" s="1">
+        <v>65</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="O2" s="1">
         <v>600000</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>1254</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="1">
         <v>500072</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="U2" s="1">
+      <c r="V2" s="1">
         <v>38</v>
       </c>
-      <c r="V2" s="1">
+      <c r="W2" s="1">
         <v>100</v>
       </c>
-      <c r="W2" s="1">
+      <c r="X2" s="1">
         <v>169</v>
       </c>
-      <c r="X2" s="1">
+      <c r="Y2" s="1">
         <v>62</v>
       </c>
     </row>
@@ -2373,7 +2389,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
@@ -2382,7 +2398,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>93</v>
@@ -2438,7 +2454,7 @@
         <v>45</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>50</v>
@@ -2546,7 +2562,7 @@
         <v>87</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>17</v>
@@ -2674,8 +2690,8 @@
   <sheetPr/>
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>
@@ -2768,19 +2784,19 @@
         <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F2" s="1">
         <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>50</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J2" s="1">
         <v>600000</v>
@@ -2813,6 +2829,465 @@
         <v>169</v>
       </c>
       <c r="T2" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1"/>
+    <row r="4" customFormat="1"/>
+    <row r="5" customFormat="1"/>
+    <row r="6" customFormat="1"/>
+    <row r="7" customFormat="1"/>
+    <row r="8" customFormat="1"/>
+    <row r="9" customFormat="1" ht="15" customHeight="1"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="sangeethanulu@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="22.6" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="4" width="30.4" customWidth="1"/>
+    <col min="5" max="5" width="26.3" customWidth="1"/>
+    <col min="7" max="7" width="10.4" customWidth="1"/>
+    <col min="8" max="8" width="7.6" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="11" max="12" width="11.4" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="16" max="16" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1">
+        <v>40</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>600000</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1254</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M2" s="1">
+        <v>500072</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O2" s="1">
+        <v>38</v>
+      </c>
+      <c r="P2" s="1">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>169</v>
+      </c>
+      <c r="R2" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1"/>
+    <row r="4" customFormat="1"/>
+    <row r="5" customFormat="1"/>
+    <row r="6" customFormat="1"/>
+    <row r="7" customFormat="1"/>
+    <row r="8" customFormat="1"/>
+    <row r="9" customFormat="1" ht="15" customHeight="1"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="sangeethanulu@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="22.6" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="4" width="30.4" customWidth="1"/>
+    <col min="5" max="5" width="26.3" customWidth="1"/>
+    <col min="7" max="7" width="16.7" customWidth="1"/>
+    <col min="8" max="8" width="7.6" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="11" max="12" width="11.4" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="16" max="16" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1">
+        <v>40</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1">
+        <v>600000</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1254</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M2" s="1">
+        <v>500072</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O2" s="1">
+        <v>38</v>
+      </c>
+      <c r="P2" s="1">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>169</v>
+      </c>
+      <c r="R2" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1"/>
+    <row r="4" customFormat="1"/>
+    <row r="5" customFormat="1"/>
+    <row r="6" customFormat="1"/>
+    <row r="7" customFormat="1"/>
+    <row r="8" customFormat="1"/>
+    <row r="9" customFormat="1" ht="15" customHeight="1"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="sangeethanulu@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:S9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="22.6" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="4" width="30.4" customWidth="1"/>
+    <col min="5" max="5" width="26.3" customWidth="1"/>
+    <col min="7" max="8" width="16.7" customWidth="1"/>
+    <col min="9" max="9" width="7.6" customWidth="1"/>
+    <col min="10" max="10" width="18.5" customWidth="1"/>
+    <col min="12" max="13" width="11.4" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="17" max="17" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1">
+        <v>40</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>600000</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1254</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="N2" s="1">
+        <v>500072</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="P2" s="1">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>100</v>
+      </c>
+      <c r="R2" s="1">
+        <v>169</v>
+      </c>
+      <c r="S2" s="1">
         <v>62</v>
       </c>
     </row>
@@ -2939,13 +3414,164 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="22.6" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="4" width="30.4" customWidth="1"/>
+    <col min="5" max="5" width="26.3" customWidth="1"/>
+    <col min="7" max="7" width="16.7" customWidth="1"/>
+    <col min="8" max="8" width="7.6" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="11" max="12" width="11.4" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="16" max="16" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="1">
+        <v>40</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="1">
+        <v>600000</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1254</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M2" s="1">
+        <v>500072</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O2" s="1">
+        <v>38</v>
+      </c>
+      <c r="P2" s="1">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>169</v>
+      </c>
+      <c r="R2" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1"/>
+    <row r="4" customFormat="1"/>
+    <row r="5" customFormat="1"/>
+    <row r="6" customFormat="1"/>
+    <row r="7" customFormat="1"/>
+    <row r="8" customFormat="1"/>
+    <row r="9" customFormat="1" ht="15" customHeight="1"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="sangeethanulu@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelCol="6"/>

</xml_diff>

<commit_message>
added corona rakshak code
</commit_message>
<xml_diff>
--- a/src/test/java/Testdata/Testdata.xlsx
+++ b/src/test/java/Testdata/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="500" firstSheet="1" activeTab="6"/>
+    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="500" firstSheet="14" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="StarProduct" sheetId="2" r:id="rId1"/>
@@ -27,13 +27,14 @@
     <sheet name="SCCPP" sheetId="20" r:id="rId18"/>
     <sheet name="SFDIP" sheetId="21" r:id="rId19"/>
     <sheet name="microrural" sheetId="22" r:id="rId20"/>
+    <sheet name="coronarakshak" sheetId="23" r:id="rId21"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="150">
   <si>
     <t>useremail</t>
   </si>
@@ -471,6 +472,18 @@
   </si>
   <si>
     <t>2 Lakhs</t>
+  </si>
+  <si>
+    <t>policyperiod</t>
+  </si>
+  <si>
+    <t>Corona Rakshak</t>
+  </si>
+  <si>
+    <t>6.5 months</t>
+  </si>
+  <si>
+    <t>1 Lakh</t>
   </si>
 </sst>
 </file>
@@ -478,12 +491,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="178" formatCode="dd/mmm"/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="180" formatCode="dd/mmm"/>
+    <numFmt numFmtId="181" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="182" formatCode="h:mm\ AM/PM"/>
   </numFmts>
   <fonts count="25">
@@ -497,7 +510,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -505,7 +518,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -546,8 +559,25 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -561,6 +591,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -568,14 +621,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -584,7 +652,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -598,7 +666,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -614,61 +682,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -695,7 +708,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -707,13 +822,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -725,43 +840,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -773,13 +870,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -791,85 +882,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -973,11 +986,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1006,43 +1025,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1062,6 +1049,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1070,161 +1072,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1240,7 +1254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -1575,156 +1589,156 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.6" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="23.875" style="11" customWidth="1"/>
-    <col min="2" max="2" width="8.5" style="11" customWidth="1"/>
-    <col min="3" max="4" width="24.375" style="11" customWidth="1"/>
-    <col min="5" max="5" width="23.875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="4" style="11" customWidth="1"/>
-    <col min="7" max="7" width="14.875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="12.375" style="11" customWidth="1"/>
-    <col min="9" max="10" width="9.25" style="11" customWidth="1"/>
-    <col min="11" max="11" width="8.875" style="11"/>
-    <col min="12" max="12" width="10" style="11" customWidth="1"/>
-    <col min="13" max="13" width="20.25" style="11" customWidth="1"/>
-    <col min="14" max="14" width="11.125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="6" style="11" customWidth="1"/>
-    <col min="16" max="16" width="4.375" style="11" customWidth="1"/>
-    <col min="17" max="17" width="9.875" style="11" customWidth="1"/>
-    <col min="18" max="18" width="11.875" style="11" customWidth="1"/>
-    <col min="19" max="19" width="12.75" style="11" customWidth="1"/>
-    <col min="20" max="20" width="10.875" style="11" customWidth="1"/>
-    <col min="21" max="25" width="8.875" style="11"/>
-    <col min="26" max="26" width="16.625" style="11" customWidth="1"/>
-    <col min="27" max="27" width="12.5" style="11" customWidth="1"/>
-    <col min="28" max="28" width="25.875" style="11" customWidth="1"/>
-    <col min="29" max="29" width="8.5" style="11" customWidth="1"/>
-    <col min="30" max="30" width="15.875" style="11" customWidth="1"/>
-    <col min="31" max="32" width="8.875" style="11"/>
-    <col min="33" max="36" width="14.625" style="11" customWidth="1"/>
-    <col min="37" max="16384" width="8.875" style="11"/>
+    <col min="1" max="1" width="23.875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="12" customWidth="1"/>
+    <col min="3" max="4" width="24.375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="23.875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="4" style="12" customWidth="1"/>
+    <col min="7" max="7" width="14.875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="12.375" style="12" customWidth="1"/>
+    <col min="9" max="10" width="9.25" style="12" customWidth="1"/>
+    <col min="11" max="11" width="8.875" style="12"/>
+    <col min="12" max="12" width="10" style="12" customWidth="1"/>
+    <col min="13" max="13" width="20.25" style="12" customWidth="1"/>
+    <col min="14" max="14" width="11.125" style="12" customWidth="1"/>
+    <col min="15" max="15" width="6" style="12" customWidth="1"/>
+    <col min="16" max="16" width="4.375" style="12" customWidth="1"/>
+    <col min="17" max="17" width="9.875" style="12" customWidth="1"/>
+    <col min="18" max="18" width="11.875" style="12" customWidth="1"/>
+    <col min="19" max="19" width="12.75" style="12" customWidth="1"/>
+    <col min="20" max="20" width="10.875" style="12" customWidth="1"/>
+    <col min="21" max="25" width="8.875" style="12"/>
+    <col min="26" max="26" width="16.625" style="12" customWidth="1"/>
+    <col min="27" max="27" width="12.5" style="12" customWidth="1"/>
+    <col min="28" max="28" width="25.875" style="12" customWidth="1"/>
+    <col min="29" max="29" width="8.5" style="12" customWidth="1"/>
+    <col min="30" max="30" width="15.875" style="12" customWidth="1"/>
+    <col min="31" max="32" width="8.875" style="12"/>
+    <col min="33" max="36" width="14.625" style="12" customWidth="1"/>
+    <col min="37" max="16384" width="8.875" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="R1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="S1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="26" t="s">
+      <c r="T1" s="27" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="25">
         <v>30</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="12">
         <v>500040</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="11">
+      <c r="P2" s="12">
         <v>23</v>
       </c>
-      <c r="Q2" s="11">
+      <c r="Q2" s="12">
         <v>123</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="R2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="S2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="T2" s="11">
+      <c r="T2" s="12">
         <v>500040</v>
       </c>
     </row>
@@ -1811,7 +1825,7 @@
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1948,7 +1962,7 @@
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2117,7 +2131,7 @@
       </c>
     </row>
     <row r="2" spans="1:25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2289,7 +2303,7 @@
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2450,7 +2464,7 @@
       </c>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2620,7 +2634,7 @@
       </c>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2706,7 +2720,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>
@@ -2786,7 +2800,7 @@
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2943,7 +2957,7 @@
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -3094,7 +3108,7 @@
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -3248,7 +3262,7 @@
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -3347,75 +3361,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:73">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="BH1" s="21"/>
-      <c r="BI1" s="21"/>
-      <c r="BJ1" s="21"/>
-      <c r="BK1" s="21"/>
-      <c r="BL1" s="21"/>
-      <c r="BM1" s="21"/>
-      <c r="BN1" s="21"/>
-      <c r="BO1" s="21"/>
-      <c r="BP1" s="21"/>
-      <c r="BQ1" s="21"/>
-      <c r="BR1" s="21"/>
-      <c r="BS1" s="21"/>
-      <c r="BT1" s="21"/>
-      <c r="BU1" s="21"/>
+      <c r="BH1" s="22"/>
+      <c r="BI1" s="22"/>
+      <c r="BJ1" s="22"/>
+      <c r="BK1" s="22"/>
+      <c r="BL1" s="22"/>
+      <c r="BM1" s="22"/>
+      <c r="BN1" s="22"/>
+      <c r="BO1" s="22"/>
+      <c r="BP1" s="22"/>
+      <c r="BQ1" s="22"/>
+      <c r="BR1" s="22"/>
+      <c r="BS1" s="22"/>
+      <c r="BT1" s="22"/>
+      <c r="BU1" s="22"/>
     </row>
     <row r="2" ht="16.35" spans="1:73">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="17">
         <v>9533679769</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="AA2" s="19"/>
-      <c r="AL2" s="20"/>
-      <c r="AP2" s="19"/>
-      <c r="BH2" s="22"/>
-      <c r="BI2" s="22"/>
-      <c r="BJ2" s="22"/>
-      <c r="BK2" s="22"/>
-      <c r="BL2" s="22"/>
-      <c r="BM2" s="22"/>
-      <c r="BN2" s="22"/>
-      <c r="BO2" s="22"/>
-      <c r="BP2" s="22"/>
-      <c r="BQ2" s="22"/>
-      <c r="BR2" s="22"/>
-      <c r="BS2" s="22"/>
-      <c r="BT2" s="22"/>
-      <c r="BU2" s="22"/>
+      <c r="AA2" s="20"/>
+      <c r="AL2" s="21"/>
+      <c r="AP2" s="20"/>
+      <c r="BH2" s="23"/>
+      <c r="BI2" s="23"/>
+      <c r="BJ2" s="23"/>
+      <c r="BK2" s="23"/>
+      <c r="BL2" s="23"/>
+      <c r="BM2" s="23"/>
+      <c r="BN2" s="23"/>
+      <c r="BO2" s="23"/>
+      <c r="BP2" s="23"/>
+      <c r="BQ2" s="23"/>
+      <c r="BR2" s="23"/>
+      <c r="BS2" s="23"/>
+      <c r="BT2" s="23"/>
+      <c r="BU2" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3509,7 +3523,7 @@
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -3580,13 +3594,194 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:W9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="3" max="4" width="26.1" customWidth="1"/>
+    <col min="6" max="6" width="14.6" customWidth="1"/>
+    <col min="7" max="7" width="21.6" customWidth="1"/>
+    <col min="8" max="9" width="16.2" customWidth="1"/>
+    <col min="22" max="22" width="11.8" customWidth="1"/>
+    <col min="23" max="23" width="21.6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="U1" t="s">
+        <v>115</v>
+      </c>
+      <c r="V1" t="s">
+        <v>116</v>
+      </c>
+      <c r="W1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="1">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="I2" s="4">
+        <v>500072</v>
+      </c>
+      <c r="J2" s="1">
+        <v>600000</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1254</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="O2" s="1">
+        <v>500072</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>38</v>
+      </c>
+      <c r="R2" s="1">
+        <v>100</v>
+      </c>
+      <c r="S2" s="1">
+        <v>169</v>
+      </c>
+      <c r="T2" s="1">
+        <v>62</v>
+      </c>
+      <c r="U2" t="s">
+        <v>119</v>
+      </c>
+      <c r="V2" t="s">
+        <v>120</v>
+      </c>
+      <c r="W2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1"/>
+    <row r="4" customFormat="1"/>
+    <row r="5" customFormat="1"/>
+    <row r="6" customFormat="1"/>
+    <row r="7" customFormat="1"/>
+    <row r="8" customFormat="1"/>
+    <row r="9" customFormat="1" spans="21:21">
+      <c r="U9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="sangeethanulu@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelCol="6"/>
@@ -3601,271 +3796,271 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
     </row>
     <row r="19" ht="16.35" spans="1:7">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3879,7 +4074,7 @@
   <sheetPr/>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -3946,7 +4141,7 @@
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -4069,7 +4264,7 @@
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -4223,7 +4418,7 @@
       </c>
     </row>
     <row r="2" spans="1:23">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -4305,8 +4500,8 @@
   <sheetPr/>
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>
@@ -4388,7 +4583,7 @@
       </c>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -4534,7 +4729,7 @@
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -4669,7 +4864,7 @@
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -4723,7 +4918,7 @@
       <c r="R2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="6">
         <v>44102</v>
       </c>
       <c r="T2" s="1" t="s">

</xml_diff>

<commit_message>
modifications in corona rakshak class
</commit_message>
<xml_diff>
--- a/src/test/java/Testdata/Testdata.xlsx
+++ b/src/test/java/Testdata/Testdata.xlsx
@@ -480,7 +480,7 @@
     <t>Corona Rakshak</t>
   </si>
   <si>
-    <t>6.5 months</t>
+    <t>3.5 months</t>
   </si>
   <si>
     <t>1 Lakh</t>
@@ -3600,7 +3600,7 @@
   <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>

</xml_diff>

<commit_message>
modifications in outpatient care
</commit_message>
<xml_diff>
--- a/src/test/java/Testdata/Testdata.xlsx
+++ b/src/test/java/Testdata/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="500" firstSheet="7" activeTab="13"/>
+    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="500" firstSheet="14" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="StarProduct" sheetId="2" r:id="rId1"/>
@@ -492,12 +492,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="180" formatCode="dd/mmm"/>
-    <numFmt numFmtId="181" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="182" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="177" formatCode="dd/mmm"/>
+    <numFmt numFmtId="178" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="182" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -559,25 +559,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -591,7 +581,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -602,36 +615,6 @@
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -651,8 +634,24 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -665,8 +664,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -675,13 +682,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -708,7 +708,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -720,7 +756,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,7 +768,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -744,55 +858,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -810,85 +882,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -986,17 +986,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1021,15 +1015,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1073,6 +1058,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1086,148 +1086,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1238,7 +1238,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1254,8 +1254,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2379,7 +2379,7 @@
   <sheetPr/>
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -2549,8 +2549,8 @@
   <sheetPr/>
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6"/>

</xml_diff>